<commit_message>
Add ability to delete remote responses
</commit_message>
<xml_diff>
--- a/tools/import_grs/grs_1.xlsx
+++ b/tools/import_grs/grs_1.xlsx
@@ -12,60 +12,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>label</t>
-  </si>
-  <si>
-    <t>short_label</t>
   </si>
   <si>
     <t>United States</t>
   </si>
   <si>
-    <t>U.S.</t>
-  </si>
-  <si>
     <t>Australia</t>
-  </si>
-  <si>
-    <t>AU</t>
   </si>
   <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>U.K.</t>
-  </si>
-  <si>
     <t>Philippines</t>
-  </si>
-  <si>
-    <t>Phil</t>
   </si>
   <si>
     <t>Kansas City</t>
   </si>
   <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>Townsville</t>
-  </si>
-  <si>
-    <t>TV</t>
-  </si>
-  <si>
     <t>Manchester</t>
-  </si>
-  <si>
-    <t>MC</t>
   </si>
   <si>
     <t>Manilla</t>
   </si>
   <si>
-    <t>ML</t>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Mexico City</t>
   </si>
 </sst>
 </file>
@@ -212,9 +188,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -225,6 +198,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1316,109 +1292,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="19.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.8516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8516" style="1" customWidth="1"/>
+    <col min="4" max="256" width="11.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -1432,7 +1376,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1440,101 +1384,70 @@
   <cols>
     <col min="1" max="1" width="19.5" style="10" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.8516" style="10" customWidth="1"/>
     <col min="4" max="4" width="11.8516" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.8516" style="10" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="10" customWidth="1"/>
+    <col min="5" max="256" width="11.8516" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
-      </c>
+      <c r="B1" s="7"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>16</v>
+        <v>8</v>
       </c>
-      <c r="B5" t="s" s="2">
-        <v>17</v>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" t="s" s="2">
+        <v>9</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>

</xml_diff>